<commit_message>
Minor update to $ALK
</commit_message>
<xml_diff>
--- a/$ALK.xlsx
+++ b/$ALK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189484CB-1F3B-46BD-B8FB-1CCBEF2ADA58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8CD5B7-D6BE-4E6E-A256-2FE0FBF97730}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E86BE7E4-A27E-4A48-9D56-E0E9F21BCB33}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{E86BE7E4-A27E-4A48-9D56-E0E9F21BCB33}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="130">
   <si>
     <t>$ALK</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>LT Debt</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
   </si>
 </sst>
 </file>
@@ -668,6 +671,25 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -683,12 +705,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -701,23 +717,10 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1101,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD178E24-23A6-43D6-9998-846D9F3D09BF}">
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1122,24 +1125,24 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="F5" s="36" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="F5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="38"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
@@ -1214,7 +1217,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="9">
-        <f>'Financial Model'!V89</f>
+        <f>'Financial Model'!V90</f>
         <v>3425</v>
       </c>
       <c r="D9" s="7" t="str">
@@ -1238,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="9">
-        <f>'Financial Model'!V90</f>
+        <f>'Financial Model'!V91</f>
         <v>2303</v>
       </c>
       <c r="D10" s="7" t="str">
@@ -1329,11 +1332,11 @@
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
       <c r="F15" s="17"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -1410,10 +1413,10 @@
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="35"/>
+      <c r="D19" s="42"/>
       <c r="F19" s="17"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -1453,11 +1456,11 @@
       <c r="P21" s="12"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
       <c r="F22" s="17"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -1582,8 +1585,8 @@
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="17"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
       <c r="F29" s="17"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -1603,7 +1606,7 @@
       <c r="C30" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="51">
+      <c r="D30" s="38">
         <v>44378</v>
       </c>
       <c r="F30" s="17"/>
@@ -1622,10 +1625,10 @@
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="44"/>
+      <c r="D31" s="49"/>
       <c r="F31" s="17"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
@@ -1665,11 +1668,11 @@
       <c r="P33" s="12"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
       <c r="F34" s="17"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
@@ -1686,11 +1689,11 @@
       <c r="B35" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="46">
-        <f>C6/'Financial Model'!V87</f>
+      <c r="C35" s="50">
+        <f>C6/'Financial Model'!V88</f>
         <v>1.3933386917609896</v>
       </c>
-      <c r="D35" s="47"/>
+      <c r="D35" s="51"/>
       <c r="F35" s="17"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
@@ -1725,8 +1728,8 @@
       <c r="B37" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="42"/>
       <c r="F37" s="18"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
@@ -1741,18 +1744,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C37:D37"/>
     <mergeCell ref="F5:P5"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
@@ -1761,6 +1757,13 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{71CE488E-8658-45D9-9C7C-D61EE936B7B0}"/>
@@ -1774,13 +1777,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC3BB7D-0C6C-4C9B-8734-5527761D2503}">
-  <dimension ref="B1:X97"/>
+  <dimension ref="B1:X98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomRight" activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1858,19 +1861,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="2:24" s="50" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="R2" s="49">
+    <row r="2" spans="2:24" s="37" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="R2" s="36">
         <v>44377</v>
       </c>
-      <c r="T2" s="50" t="s">
+      <c r="T2" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="V2" s="49">
+      <c r="V2" s="36">
         <v>44742</v>
       </c>
     </row>
-    <row r="3" spans="2:24" s="50" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="V3" s="48">
+    <row r="3" spans="2:24" s="37" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="V3" s="35">
         <v>44378</v>
       </c>
     </row>
@@ -1921,7 +1924,7 @@
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="26" t="s">
         <v>59</v>
       </c>
       <c r="R8" s="29">
@@ -1932,7 +1935,7 @@
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="26" t="s">
         <v>60</v>
       </c>
       <c r="R9" s="29">
@@ -1943,7 +1946,7 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="26" t="s">
         <v>61</v>
       </c>
       <c r="R10" s="29">
@@ -1954,7 +1957,7 @@
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="26" t="s">
         <v>62</v>
       </c>
       <c r="R11" s="29">
@@ -1965,7 +1968,7 @@
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="26" t="s">
         <v>63</v>
       </c>
       <c r="R12" s="29">
@@ -1976,7 +1979,7 @@
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="26" t="s">
         <v>64</v>
       </c>
       <c r="R13" s="29">
@@ -1987,7 +1990,7 @@
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="26" t="s">
         <v>65</v>
       </c>
       <c r="R14" s="29">
@@ -1998,7 +2001,7 @@
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="26" t="s">
         <v>66</v>
       </c>
       <c r="R15" s="29">
@@ -2009,7 +2012,7 @@
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="26" t="s">
         <v>67</v>
       </c>
       <c r="R16" s="29">
@@ -2019,47 +2022,49 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R17" s="30">
+      <c r="R17" s="29">
         <f>SUM(R8:R16)</f>
         <v>718</v>
       </c>
-      <c r="V17" s="30">
+      <c r="V17" s="29">
         <f>SUM(V8:V16)</f>
         <v>1944</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R18" s="29">
-        <v>98</v>
-      </c>
-      <c r="V18" s="29">
-        <v>104</v>
+    <row r="18" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" s="30">
+        <f>R7-R17</f>
+        <v>809</v>
+      </c>
+      <c r="V18" s="30">
+        <f>V7-V17</f>
+        <v>714</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R19" s="29">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="V19" s="29">
-        <v>50</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R20" s="29">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="V20" s="29">
         <v>50</v>
@@ -2067,782 +2072,793 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R21" s="29">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="V21" s="29">
-        <v>177</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R22" s="29">
-        <v>-4</v>
+        <v>117</v>
       </c>
       <c r="V22" s="29">
-        <v>146</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R23" s="29">
-        <v>-23</v>
+        <v>-4</v>
       </c>
       <c r="V23" s="29">
-        <v>0</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R24" s="29">
+        <v>-23</v>
+      </c>
+      <c r="V24" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="R24" s="29">
-        <f>SUM(R17:R23)</f>
+      <c r="R25" s="29">
+        <f>SUM(R19:R24)+R17</f>
         <v>978</v>
       </c>
-      <c r="V24" s="29">
-        <f>SUM(V17:V23)</f>
+      <c r="V25" s="29">
+        <f>SUM(V19:V24)+V17</f>
         <v>2471</v>
       </c>
     </row>
-    <row r="25" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="R25" s="30">
-        <f>R7-R24</f>
+      <c r="R26" s="30">
+        <f>R7-R25</f>
         <v>549</v>
       </c>
-      <c r="V25" s="30">
-        <f>V7-V24</f>
+      <c r="V26" s="30">
+        <f>V7-V25</f>
         <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R26" s="29">
-        <v>6</v>
-      </c>
-      <c r="V26" s="29">
-        <v>11</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R27" s="29">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="V27" s="29">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R28" s="29">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="V28" s="29">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R29" s="29">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="V29" s="29">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R30" s="29">
-        <f>R26-R27+R28+R29</f>
-        <v>-21</v>
+        <v>9</v>
       </c>
       <c r="V30" s="29">
-        <f>V26-V27+V28+V29</f>
-        <v>-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R31" s="29">
-        <f>R25+R30</f>
-        <v>528</v>
+        <f>R27-R28+R29+R30</f>
+        <v>-21</v>
       </c>
       <c r="V31" s="29">
-        <f>V25+V30</f>
-        <v>185</v>
+        <f>V27-V28+V29+V30</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R32" s="29">
+        <f>R26+R31</f>
+        <v>528</v>
+      </c>
+      <c r="V32" s="29">
+        <f>V26+V31</f>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R32" s="29">
+      <c r="R33" s="29">
         <v>131</v>
       </c>
-      <c r="V32" s="29">
+      <c r="V33" s="29">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
+    <row r="34" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="R33" s="30">
-        <f>R31-R32</f>
+      <c r="R34" s="30">
+        <f>R32-R33</f>
         <v>397</v>
       </c>
-      <c r="V33" s="30">
-        <f>V31-V32</f>
+      <c r="V34" s="30">
+        <f>V32-V33</f>
         <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R34" s="28">
-        <f>R33/R35</f>
-        <v>3.1760762258294197</v>
-      </c>
-      <c r="V34" s="28">
-        <f>V33/V35</f>
-        <v>1.098440846194574</v>
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R35" s="28">
+        <f>R34/R36</f>
+        <v>3.1760762258294197</v>
+      </c>
+      <c r="V35" s="28">
+        <f>V34/V36</f>
+        <v>1.098440846194574</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R35" s="27">
+      <c r="R36" s="27">
         <v>124.997</v>
       </c>
-      <c r="V35" s="27">
+      <c r="V36" s="27">
         <v>126.54300000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+    <row r="39" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="V38" s="32">
+      <c r="V39" s="32">
         <f>V7/R7-1</f>
         <v>0.74066797642436155</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="R41" s="31">
-        <f>R17/R7</f>
-        <v>0.47020301244269808</v>
-      </c>
-      <c r="V41" s="31">
-        <f>V17/V7</f>
-        <v>0.73137697516930023</v>
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R42" s="31">
-        <f>R25/R7</f>
-        <v>0.35952848722986247</v>
+        <f>R18/R7</f>
+        <v>0.52979698755730187</v>
       </c>
       <c r="V42" s="31">
-        <f>V25/V7</f>
-        <v>7.0353649360421364E-2</v>
+        <f>V18/V7</f>
+        <v>0.26862302483069977</v>
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R43" s="31">
-        <f>R33/R7</f>
-        <v>0.25998690242305172</v>
+        <f>R26/R7</f>
+        <v>0.35952848722986247</v>
       </c>
       <c r="V43" s="31">
-        <f>V33/V7</f>
-        <v>5.2294958615500375E-2</v>
+        <f>V26/V7</f>
+        <v>7.0353649360421364E-2</v>
       </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R44" s="31">
+        <f>R34/R7</f>
+        <v>0.25998690242305172</v>
+      </c>
+      <c r="V44" s="31">
+        <f>V34/V7</f>
+        <v>5.2294958615500375E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R44" s="31">
-        <f>R32/R31</f>
+      <c r="R45" s="31">
+        <f>R33/R32</f>
         <v>0.24810606060606061</v>
       </c>
-      <c r="V44" s="31">
-        <f>V32/V31</f>
+      <c r="V45" s="31">
+        <f>V33/V32</f>
         <v>0.24864864864864866</v>
       </c>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B48" s="33" t="s">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B49" s="33" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="T49" s="30">
-        <v>470</v>
-      </c>
-      <c r="U49" s="30"/>
-      <c r="V49" s="30">
-        <v>778</v>
       </c>
     </row>
     <row r="50" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="T50" s="30">
-        <v>2646</v>
+        <v>470</v>
       </c>
       <c r="U50" s="30"/>
       <c r="V50" s="30">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="T51" s="30">
+        <v>2646</v>
+      </c>
+      <c r="U51" s="30"/>
+      <c r="V51" s="30">
         <v>2647</v>
-      </c>
-    </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="T51" s="29">
-        <v>546</v>
-      </c>
-      <c r="U51" s="29"/>
-      <c r="V51" s="29">
-        <v>401</v>
       </c>
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T52" s="29">
-        <v>62</v>
+        <v>546</v>
       </c>
       <c r="U52" s="29"/>
       <c r="V52" s="29">
-        <v>93</v>
+        <v>401</v>
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T53" s="29">
-        <v>196</v>
+        <v>62</v>
       </c>
       <c r="U53" s="29"/>
       <c r="V53" s="29">
-        <v>313</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T54" s="29">
-        <f>SUM(T49:T53)</f>
-        <v>3920</v>
+        <v>196</v>
       </c>
       <c r="U54" s="29"/>
       <c r="V54" s="29">
-        <f>SUM(V49:V53)</f>
-        <v>4232</v>
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B55" s="26" t="s">
-        <v>99</v>
+      <c r="B55" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="T55" s="29">
-        <v>8127</v>
+        <f>SUM(T50:T54)</f>
+        <v>3920</v>
       </c>
       <c r="U55" s="29"/>
       <c r="V55" s="29">
-        <v>8569</v>
+        <f>SUM(V50:V54)</f>
+        <v>4232</v>
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B56" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T56" s="29">
-        <v>1489</v>
+        <v>8127</v>
       </c>
       <c r="U56" s="29"/>
       <c r="V56" s="29">
-        <v>1532</v>
+        <v>8569</v>
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B57" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T57" s="29">
-        <v>384</v>
+        <v>1489</v>
       </c>
       <c r="U57" s="29"/>
       <c r="V57" s="29">
-        <v>292</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
-        <v>98</v>
+      <c r="B58" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="T58" s="29">
-        <f>SUM(T55:T57)</f>
-        <v>10000</v>
+        <v>384</v>
       </c>
       <c r="U58" s="29"/>
       <c r="V58" s="29">
-        <f>SUM(V55:V57)</f>
-        <v>10393</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B59" s="26" t="s">
-        <v>102</v>
+      <c r="B59" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="T59" s="29">
-        <v>3862</v>
+        <f>SUM(T56:T58)</f>
+        <v>10000</v>
       </c>
       <c r="U59" s="29"/>
       <c r="V59" s="29">
-        <v>3922</v>
+        <f>SUM(V56:V58)</f>
+        <v>10393</v>
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
-        <v>103</v>
+      <c r="B60" s="26" t="s">
+        <v>102</v>
       </c>
       <c r="T60" s="29">
-        <f>T58-T59</f>
-        <v>6138</v>
+        <v>3862</v>
       </c>
       <c r="U60" s="29"/>
       <c r="V60" s="29">
-        <f>V58-V59</f>
-        <v>6471</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B61" s="26" t="s">
-        <v>104</v>
+      <c r="B61" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="T61" s="29">
-        <v>1453</v>
+        <f>T59-T60</f>
+        <v>6138</v>
       </c>
       <c r="U61" s="29"/>
       <c r="V61" s="29">
-        <v>1669</v>
+        <f>V59-V60</f>
+        <v>6471</v>
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B62" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T62" s="29">
-        <v>2044</v>
+        <v>1453</v>
       </c>
       <c r="U62" s="29"/>
       <c r="V62" s="29">
-        <v>2041</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="63" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B63" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T63" s="29">
-        <v>396</v>
+        <v>2044</v>
       </c>
       <c r="U63" s="29"/>
       <c r="V63" s="29">
-        <v>387</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
-        <v>107</v>
+      <c r="B64" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="T64" s="29">
-        <f>SUM(T61:T63)</f>
-        <v>3893</v>
+        <v>396</v>
       </c>
       <c r="U64" s="29"/>
       <c r="V64" s="29">
-        <f>SUM(V61:V63)</f>
-        <v>4097</v>
+        <v>387</v>
       </c>
     </row>
     <row r="65" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T65" s="29">
-        <f>T64+T60+T54</f>
-        <v>13951</v>
+        <f>SUM(T62:T64)</f>
+        <v>3893</v>
       </c>
       <c r="U65" s="29"/>
       <c r="V65" s="29">
-        <f>V64+V60+V54</f>
+        <f>SUM(V62:V64)</f>
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="66" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="T66" s="29">
+        <f>T65+T61+T55</f>
+        <v>13951</v>
+      </c>
+      <c r="U66" s="29"/>
+      <c r="V66" s="29">
+        <f>V65+V61+V55</f>
         <v>14800</v>
       </c>
     </row>
-    <row r="66" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="T66" s="29"/>
-      <c r="U66" s="29"/>
-      <c r="V66" s="29"/>
-    </row>
     <row r="67" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="T67" s="29">
-        <v>200</v>
-      </c>
+      <c r="T67" s="29"/>
       <c r="U67" s="29"/>
-      <c r="V67" s="29">
-        <v>286</v>
-      </c>
+      <c r="V67" s="29"/>
     </row>
     <row r="68" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T68" s="29">
-        <v>457</v>
+        <v>200</v>
       </c>
       <c r="U68" s="29"/>
       <c r="V68" s="29">
-        <v>416</v>
+        <v>286</v>
       </c>
     </row>
     <row r="69" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T69" s="29">
-        <v>1163</v>
+        <v>457</v>
       </c>
       <c r="U69" s="29"/>
       <c r="V69" s="29">
-        <v>1778</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T70" s="29">
-        <v>625</v>
+        <v>1163</v>
       </c>
       <c r="U70" s="29"/>
       <c r="V70" s="29">
-        <v>794</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="71" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T71" s="29">
-        <v>912</v>
+        <v>625</v>
       </c>
       <c r="U71" s="29"/>
       <c r="V71" s="29">
-        <v>1012</v>
+        <v>794</v>
       </c>
     </row>
     <row r="72" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="T72" s="29">
-        <v>268</v>
+        <v>912</v>
       </c>
       <c r="U72" s="29"/>
       <c r="V72" s="29">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="73" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T73" s="29">
+        <v>268</v>
+      </c>
+      <c r="U73" s="29"/>
+      <c r="V73" s="29">
         <v>274</v>
       </c>
     </row>
-    <row r="73" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="2" t="s">
+    <row r="74" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="T73" s="30">
+      <c r="T74" s="30">
         <v>366</v>
       </c>
-      <c r="U73" s="30"/>
-      <c r="V73" s="30">
+      <c r="U74" s="30"/>
+      <c r="V74" s="30">
         <v>342</v>
       </c>
     </row>
-    <row r="74" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B74" s="1" t="s">
+    <row r="75" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T74" s="29">
-        <f>SUM(T67:T73)</f>
+      <c r="T75" s="29">
+        <f>SUM(T68:T74)</f>
         <v>3991</v>
       </c>
-      <c r="U74" s="29"/>
-      <c r="V74" s="29">
-        <f>SUM(V67:V73)</f>
+      <c r="U75" s="29"/>
+      <c r="V75" s="29">
+        <f>SUM(V68:V74)</f>
         <v>4902</v>
       </c>
     </row>
-    <row r="75" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="2" t="s">
+    <row r="76" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="T75" s="30">
+      <c r="T76" s="30">
         <v>2173</v>
       </c>
-      <c r="U75" s="30"/>
-      <c r="V75" s="30">
+      <c r="U76" s="30"/>
+      <c r="V76" s="30">
         <v>1961</v>
-      </c>
-    </row>
-    <row r="76" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B76" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="T76" s="29">
-        <v>1279</v>
-      </c>
-      <c r="U76" s="29"/>
-      <c r="V76" s="29">
-        <v>1505</v>
       </c>
     </row>
     <row r="77" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T77" s="29">
-        <v>578</v>
+        <v>1279</v>
       </c>
       <c r="U77" s="29"/>
       <c r="V77" s="29">
-        <v>552</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="78" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="T78" s="29">
-        <v>1446</v>
+        <v>578</v>
       </c>
       <c r="U78" s="29"/>
       <c r="V78" s="29">
-        <v>1429</v>
+        <v>552</v>
       </c>
     </row>
     <row r="79" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="T79" s="29">
-        <v>305</v>
+        <v>1446</v>
       </c>
       <c r="U79" s="29"/>
       <c r="V79" s="29">
-        <v>299</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="80" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T80" s="29">
-        <v>378</v>
+        <v>305</v>
       </c>
       <c r="U80" s="29"/>
       <c r="V80" s="29">
-        <v>353</v>
+        <v>299</v>
       </c>
     </row>
     <row r="81" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T81" s="29">
-        <f>T74+SUM(T75:T80)</f>
-        <v>10150</v>
+        <v>378</v>
       </c>
       <c r="U81" s="29"/>
       <c r="V81" s="29">
-        <f>V74+SUM(V75:V80)</f>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="82" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B82" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T82" s="29">
+        <f>T75+SUM(T76:T81)</f>
+        <v>10150</v>
+      </c>
+      <c r="U82" s="29"/>
+      <c r="V82" s="29">
+        <f>V75+SUM(V76:V81)</f>
         <v>11001</v>
       </c>
-      <c r="X81" s="29"/>
-    </row>
-    <row r="82" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="T82" s="29"/>
-      <c r="U82" s="29"/>
-      <c r="V82" s="29"/>
+      <c r="X82" s="29"/>
     </row>
     <row r="83" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B83" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="T83" s="29">
-        <v>3801</v>
-      </c>
+      <c r="T83" s="29"/>
       <c r="U83" s="29"/>
-      <c r="V83" s="29">
-        <v>3799</v>
-      </c>
+      <c r="V83" s="29"/>
     </row>
     <row r="84" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T84" s="29">
+        <v>3801</v>
+      </c>
+      <c r="U84" s="29"/>
+      <c r="V84" s="29">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="85" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B85" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T84" s="29">
-        <f>T83+T81</f>
+      <c r="T85" s="29">
+        <f>T84+T82</f>
         <v>13951</v>
       </c>
-      <c r="V84" s="29">
-        <f>V83+V81</f>
+      <c r="V85" s="29">
+        <f>V84+V82</f>
         <v>14800</v>
-      </c>
-    </row>
-    <row r="86" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="T86" s="29">
-        <f>T65-T81</f>
-        <v>3801</v>
-      </c>
-      <c r="V86" s="29">
-        <f>V65-V81</f>
-        <v>3799</v>
       </c>
     </row>
     <row r="87" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="T87" s="29">
+        <f>T66-T82</f>
+        <v>3801</v>
+      </c>
+      <c r="V87" s="29">
+        <f>V66-V82</f>
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="88" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B88" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="V87" s="1">
-        <f>V86/V35</f>
+      <c r="V88" s="1">
+        <f>V87/V36</f>
         <v>30.021415645274729</v>
-      </c>
-    </row>
-    <row r="89" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B89" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T89" s="29">
-        <f>T49+T50</f>
-        <v>3116</v>
-      </c>
-      <c r="U89" s="29"/>
-      <c r="V89" s="29">
-        <f>V49+V50</f>
-        <v>3425</v>
       </c>
     </row>
     <row r="90" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T90" s="29">
-        <f>T73+T75</f>
-        <v>2539</v>
+        <f>T50+T51</f>
+        <v>3116</v>
       </c>
       <c r="U90" s="29"/>
       <c r="V90" s="29">
-        <f>V73+V75</f>
-        <v>2303</v>
+        <f>V50+V51</f>
+        <v>3425</v>
       </c>
     </row>
     <row r="91" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T91" s="29">
-        <f t="shared" ref="T91:U91" si="0">T89-T90</f>
-        <v>577</v>
+        <f>T74+T76</f>
+        <v>2539</v>
       </c>
       <c r="U91" s="29"/>
       <c r="V91" s="29">
-        <f>V89-V90</f>
+        <f>V74+V76</f>
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="92" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T92" s="29">
+        <f t="shared" ref="T92" si="0">T90-T91</f>
+        <v>577</v>
+      </c>
+      <c r="U92" s="29"/>
+      <c r="V92" s="29">
+        <f>V90-V91</f>
         <v>1122</v>
-      </c>
-    </row>
-    <row r="93" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B93" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="V93" s="1">
-        <v>40.049999999999997</v>
       </c>
     </row>
     <row r="94" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V94" s="29">
-        <f>V93*V35</f>
-        <v>5068.0471500000003</v>
+        <v>127</v>
+      </c>
+      <c r="V94" s="1">
+        <v>40.049999999999997</v>
       </c>
     </row>
     <row r="95" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V95" s="29">
+        <f>V94*V36</f>
+        <v>5068.0471500000003</v>
+      </c>
+    </row>
+    <row r="96" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B96" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V95" s="29">
-        <f>V94-V91</f>
+      <c r="V96" s="29">
+        <f>V95-V92</f>
         <v>3946.0471500000003</v>
       </c>
     </row>
-    <row r="97" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B97" s="1" t="s">
+    <row r="98" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B98" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V97" s="45">
-        <f>V93/V87</f>
+      <c r="V98" s="34">
+        <f>V94/V88</f>
         <v>1.3340476836009476</v>
       </c>
     </row>
@@ -2851,6 +2867,7 @@
     <hyperlink ref="V1" r:id="rId1" xr:uid="{2BFDBA4F-3ED4-4AEE-A5E2-00AB0E0EF3A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
   <ignoredErrors>
     <ignoredError sqref="V7" formulaRange="1"/>
   </ignoredErrors>

</xml_diff>